<commit_message>
make some more adjustments
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Имя</t>
   </si>
@@ -95,14 +95,50 @@
     <t>SMTP сервер</t>
   </si>
   <si>
-    <t>Robot-LinqActsTask</t>
+    <t>Robot-LinqActsTask-Test</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\1cv8t\8.3.18.1741\bin\1cv8st.exe</t>
+  </si>
+  <si>
+    <t>1CFilePath</t>
+  </si>
+  <si>
+    <t>1СApplicationName</t>
+  </si>
+  <si>
+    <t>1cv8st.exe</t>
+  </si>
+  <si>
+    <t>ActsInputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\Акты_Исходные.xlsx</t>
+  </si>
+  <si>
+    <t>ActsWorkingFilePath</t>
+  </si>
+  <si>
+    <t>Data\Temp\Акты_Исходные.xlsx</t>
+  </si>
+  <si>
+    <t>ResultsWorkingPath</t>
+  </si>
+  <si>
+    <t>Data\Temp\Шаблон.xlsx</t>
+  </si>
+  <si>
+    <t>ResultsInputPath</t>
+  </si>
+  <si>
+    <t>Data\Input\Шаблон.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -168,6 +204,11 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -196,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -242,6 +283,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -525,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E544"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -625,67 +667,101 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14"/>
-      <c r="B14" s="16"/>
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjust logic in Excel and 1C scripts, finalize framework scripts, adjust naming for activities in all scripts, make some more adjustments
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Имя</t>
   </si>
@@ -95,14 +95,50 @@
     <t>SMTP сервер</t>
   </si>
   <si>
-    <t>Robot-LinqActsTask</t>
+    <t>Robot-LinqActsTask-Test</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\1cv8t\8.3.18.1741\bin\1cv8st.exe</t>
+  </si>
+  <si>
+    <t>1CFilePath</t>
+  </si>
+  <si>
+    <t>1СApplicationName</t>
+  </si>
+  <si>
+    <t>1cv8st.exe</t>
+  </si>
+  <si>
+    <t>ActsInputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\Акты_Исходные.xlsx</t>
+  </si>
+  <si>
+    <t>ActsWorkingFilePath</t>
+  </si>
+  <si>
+    <t>Data\Temp\Акты_Исходные.xlsx</t>
+  </si>
+  <si>
+    <t>ResultsWorkingPath</t>
+  </si>
+  <si>
+    <t>Data\Temp\Шаблон.xlsx</t>
+  </si>
+  <si>
+    <t>ResultsInputPath</t>
+  </si>
+  <si>
+    <t>Data\Input\Шаблон.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -168,6 +204,11 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -196,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -242,6 +283,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -525,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E544"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -625,67 +667,101 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14"/>
-      <c r="B14" s="16"/>
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>